<commit_message>
Adding homework solutions as of 11:23 on 9/23/19
</commit_message>
<xml_diff>
--- a/1. Excel Homework/Instructions/Part-1/HW_Task1_GolfingTargets/GolfingTargets.xlsx
+++ b/1. Excel Homework/Instructions/Part-1/HW_Task1_GolfingTargets/GolfingTargets.xlsx
@@ -1,23 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18067"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\GitHub\DataViz-Lesson-Plans\01-Lesson-Plans\01-Excel\3\Activities\09-Stu_GolfingTargets\Unsolved\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s01la\Desktop\GW Data Boot Camp\Lanciotti_GW_HW\1. Excel Homework\Instructions\Part-1\HW_Task1_GolfingTargets\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A7CD0D2-7061-4D67-9219-3BF536D97C5D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="12780"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -119,7 +126,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -166,6 +173,1740 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="6.987020392246554E-2"/>
+          <c:y val="3.8578574227579342E-2"/>
+          <c:w val="0.79963001705078818"/>
+          <c:h val="0.84153567579195843"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Subject 1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$21</c:f>
+              <c:strCache>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>Shot 1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Shot 2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Shot 3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Shot 4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Shot 5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Shot 6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Shot 7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Shot 8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Shot 9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Shot 10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Shot 11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Shot 12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Shot 13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Shot 14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Shot 15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Shot 16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Shot 17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Shot 18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Shot 19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>Shot 20</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$G$2:$G$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.75</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.75</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.25</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.25</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.25</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.25</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B371-4B71-B405-E4D433F99236}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Subject 2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$21</c:f>
+              <c:strCache>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>Shot 1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Shot 2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Shot 3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Shot 4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Shot 5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Shot 6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Shot 7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Shot 8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Shot 9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Shot 10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Shot 11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Shot 12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Shot 13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Shot 14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Shot 15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Shot 16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Shot 17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Shot 18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Shot 19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>Shot 20</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$H$2:$H$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10.75</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.25</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6.75</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8.5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>9.5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>10.75</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>8.25</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>10.5</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>8.75</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-B371-4B71-B405-E4D433F99236}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Subject 3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$21</c:f>
+              <c:strCache>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>Shot 1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Shot 2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Shot 3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Shot 4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Shot 5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Shot 6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Shot 7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Shot 8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Shot 9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Shot 10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Shot 11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Shot 12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Shot 13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Shot 14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Shot 15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Shot 16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Shot 17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Shot 18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Shot 19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>Shot 20</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$I$2:$I$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.75</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.75</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.25</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.75</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5.25</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6.25</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>5.75</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>6.25</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>6.75</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-B371-4B71-B405-E4D433F99236}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Subject 4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$21</c:f>
+              <c:strCache>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>Shot 1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Shot 2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Shot 3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Shot 4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Shot 5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Shot 6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Shot 7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Shot 8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Shot 9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Shot 10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Shot 11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Shot 12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Shot 13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Shot 14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Shot 15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Shot 16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Shot 17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Shot 18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Shot 19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>Shot 20</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$J$2:$J$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.75</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10.25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10.75</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10.25</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>12.25</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>10.75</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>11.5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>10.25</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>10.25</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>10.25</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>9.75</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>9.75</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>11</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-B371-4B71-B405-E4D433F99236}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Subject 5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$21</c:f>
+              <c:strCache>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>Shot 1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Shot 2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Shot 3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Shot 4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Shot 5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Shot 6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Shot 7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Shot 8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Shot 9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Shot 10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Shot 11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Shot 12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Shot 13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Shot 14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Shot 15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Shot 16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Shot 17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Shot 18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Shot 19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>Shot 20</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$K$2:$K$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15.75</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>15.75</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>15.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>15.75</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>15.25</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>15.25</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>15.25</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>15.25</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>14.5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>15.25</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>16.25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-B371-4B71-B405-E4D433F99236}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="449673864"/>
+        <c:axId val="348881384"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="449673864"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="348881384"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="348881384"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Distance to Hole</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="449673864"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>613522</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>115980</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>638735</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>151279</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{305D9057-94B6-418C-8A40-FC2F354020E9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -464,16 +2205,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:K21"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -505,7 +2246,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -524,8 +2265,23 @@
       <c r="F2">
         <v>18</v>
       </c>
+      <c r="G2" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H2" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I2" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J2" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K2" t="e">
+        <v>#N/A</v>
+      </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -544,8 +2300,23 @@
       <c r="F3">
         <v>16</v>
       </c>
+      <c r="G3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K3" t="e">
+        <v>#N/A</v>
+      </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -564,8 +2335,23 @@
       <c r="F4">
         <v>13</v>
       </c>
+      <c r="G4" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H4" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I4" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J4" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K4" t="e">
+        <v>#N/A</v>
+      </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -584,8 +2370,28 @@
       <c r="F5">
         <v>16</v>
       </c>
+      <c r="G5">
+        <f t="shared" ref="G5:G21" si="0">AVERAGE(B2:B5)</f>
+        <v>2.25</v>
+      </c>
+      <c r="H5">
+        <f t="shared" ref="H5:H21" si="1">AVERAGE(C2:C5)</f>
+        <v>10.75</v>
+      </c>
+      <c r="I5">
+        <f t="shared" ref="I5:I21" si="2">AVERAGE(D2:D5)</f>
+        <v>5.75</v>
+      </c>
+      <c r="J5">
+        <f t="shared" ref="J5:J21" si="3">AVERAGE(E2:E5)</f>
+        <v>8.75</v>
+      </c>
+      <c r="K5">
+        <f t="shared" ref="K5:K21" si="4">AVERAGE(F2:F5)</f>
+        <v>15.75</v>
+      </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -604,8 +2410,28 @@
       <c r="F6">
         <v>15</v>
       </c>
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="1"/>
+        <v>10.5</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="3"/>
+        <v>10.25</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="4"/>
+        <v>15</v>
+      </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -624,8 +2450,28 @@
       <c r="F7">
         <v>16</v>
       </c>
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>2.25</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="2"/>
+        <v>6.25</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="3"/>
+        <v>9.5</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="4"/>
+        <v>15</v>
+      </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -644,8 +2490,28 @@
       <c r="F8">
         <v>16</v>
       </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="1"/>
+        <v>8.5</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="2"/>
+        <v>6.5</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="3"/>
+        <v>9.5</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="4"/>
+        <v>15.75</v>
+      </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -664,8 +2530,28 @@
       <c r="F9">
         <v>15</v>
       </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="2"/>
+        <v>6.75</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="3"/>
+        <v>10.75</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="4"/>
+        <v>15.5</v>
+      </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -684,8 +2570,28 @@
       <c r="F10">
         <v>16</v>
       </c>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>1.75</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="1"/>
+        <v>8.25</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="2"/>
+        <v>6.25</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="3"/>
+        <v>10.25</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="4"/>
+        <v>15.75</v>
+      </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -704,8 +2610,28 @@
       <c r="F11">
         <v>14</v>
       </c>
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>2.75</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="3"/>
+        <v>12.25</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="4"/>
+        <v>15.25</v>
+      </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -724,8 +2650,28 @@
       <c r="F12">
         <v>16</v>
       </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="3"/>
+        <v>12.5</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="4"/>
+        <v>15.25</v>
+      </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -744,8 +2690,28 @@
       <c r="F13">
         <v>14</v>
       </c>
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="1"/>
+        <v>6.75</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="2"/>
+        <v>4.75</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="3"/>
+        <v>10.75</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="4"/>
+        <v>15</v>
+      </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -764,8 +2730,28 @@
       <c r="F14">
         <v>17</v>
       </c>
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>2.25</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="2"/>
+        <v>5.25</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="3"/>
+        <v>11.5</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="4"/>
+        <v>15.25</v>
+      </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -784,8 +2770,28 @@
       <c r="F15">
         <v>14</v>
       </c>
+      <c r="G15">
+        <f t="shared" si="0"/>
+        <v>2.25</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="1"/>
+        <v>8.5</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="3"/>
+        <v>10.25</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="4"/>
+        <v>15.25</v>
+      </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -804,8 +2810,28 @@
       <c r="F16">
         <v>13</v>
       </c>
+      <c r="G16">
+        <f t="shared" si="0"/>
+        <v>3.25</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="1"/>
+        <v>9.5</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="2"/>
+        <v>6.25</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="3"/>
+        <v>10.25</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="4"/>
+        <v>14.5</v>
+      </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -824,8 +2850,28 @@
       <c r="F17">
         <v>17</v>
       </c>
+      <c r="G17">
+        <f t="shared" si="0"/>
+        <v>3.25</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="1"/>
+        <v>10.75</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="2"/>
+        <v>5.5</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="3"/>
+        <v>10.25</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="4"/>
+        <v>15.25</v>
+      </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -844,8 +2890,28 @@
       <c r="F18">
         <v>16</v>
       </c>
+      <c r="G18">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="1"/>
+        <v>8.25</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="2"/>
+        <v>5.75</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="3"/>
+        <v>9.75</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="4"/>
+        <v>15</v>
+      </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -864,8 +2930,28 @@
       <c r="F19">
         <v>14</v>
       </c>
+      <c r="G19">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="1"/>
+        <v>10.5</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="3"/>
+        <v>9.75</v>
+      </c>
+      <c r="K19">
+        <f t="shared" si="4"/>
+        <v>15</v>
+      </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -884,8 +2970,28 @@
       <c r="F20">
         <v>17</v>
       </c>
+      <c r="G20">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="2"/>
+        <v>6.25</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="3"/>
+        <v>11</v>
+      </c>
+      <c r="K20">
+        <f t="shared" si="4"/>
+        <v>16</v>
+      </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -903,9 +3009,30 @@
       </c>
       <c r="F21">
         <v>18</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="1"/>
+        <v>8.75</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="2"/>
+        <v>6.75</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="3"/>
+        <v>11</v>
+      </c>
+      <c r="K21">
+        <f t="shared" si="4"/>
+        <v>16.25</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>